<commit_message>
elc, top -> left, right
</commit_message>
<xml_diff>
--- a/research/Astrophysics_Personal_Glossary_Notebook.xlsx
+++ b/research/Astrophysics_Personal_Glossary_Notebook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="28455" windowHeight="12030" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="28455" windowHeight="12030" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Orbital Period" sheetId="1" r:id="rId1"/>
@@ -15,15 +15,16 @@
     <sheet name=" TIC 178155732" sheetId="6" r:id="rId6"/>
     <sheet name="Orbit glossary" sheetId="7" r:id="rId7"/>
     <sheet name="Kepler Parameter 6" sheetId="9" r:id="rId8"/>
-    <sheet name="Konvertierungsbeispiele" sheetId="11" r:id="rId9"/>
-    <sheet name="Exoplanetenparameterableitung" sheetId="12" r:id="rId10"/>
+    <sheet name="Demo" sheetId="13" r:id="rId9"/>
+    <sheet name="Konvertierungsbeispiele" sheetId="11" r:id="rId10"/>
+    <sheet name="Exoplanetenparameterableitung" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="125725" calcOnSave="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="278">
   <si>
     <t>DT</t>
   </si>
@@ -1187,6 +1188,15 @@
   </si>
   <si>
     <t>Angle in the plane of the orbit between the direction of periapsis and the current position of the body, as seen from the main focus of the ellipse (the point around which the object orbits).</t>
+  </si>
+  <si>
+    <t>Checken!!!!</t>
+  </si>
+  <si>
+    <t>nein 270 ist woanders</t>
+  </si>
+  <si>
+    <t>Mean longitude is the ecliptic longitude at which an orbiting body could be found if its orbit were circular and free of perturbations. While nominally a simple longitude, in practice the mean longitude does not correspond to any one physical angle.</t>
   </si>
 </sst>
 </file>
@@ -1370,7 +1380,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -1510,6 +1520,166 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1520,7 +1690,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1680,6 +1850,62 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -5110,8 +5336,8 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>309984</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>371475</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>561975</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5174,6 +5400,2403 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>503850</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>56175</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="53" name="Ellipse 52"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5743575" y="6648450"/>
+          <a:ext cx="180000" cy="180000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>160950</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>56175</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="54" name="Ellipse 53"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5400675" y="3981450"/>
+          <a:ext cx="180000" cy="180000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>761999</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>677999</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>106500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Ellipse 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1523999" y="952500"/>
+          <a:ext cx="1440000" cy="1440000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>689310</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>50132</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>600296</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>174178</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Ellipse 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21606711" y="1090362"/>
+          <a:ext cx="1439999" cy="1440000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>20775</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Ellipse 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4676775" y="1685925"/>
+          <a:ext cx="1440000" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>724401</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>67894</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>127051</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Ellipse 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22982822" y="683294"/>
+          <a:ext cx="108000" cy="108000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>704849</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>50849</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>22275</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Ellipse 18"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6038849" y="1628775"/>
+          <a:ext cx="108000" cy="108000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>619124</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>727124</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>22275</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="Ellipse 19"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2905124" y="1628775"/>
+          <a:ext cx="108000" cy="108000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>761999</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>677999</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>106500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="Ellipse 20"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1609724" y="676275"/>
+          <a:ext cx="1440000" cy="1440000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>20775</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="Ellipse 21"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4762500" y="1409700"/>
+          <a:ext cx="1440000" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>127049</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>22275</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="Ellipse 22"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5438774" y="4019550"/>
+          <a:ext cx="108000" cy="108000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>666749</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>12749</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>60375</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="Ellipse 23"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2276474" y="3295650"/>
+          <a:ext cx="108000" cy="108000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>135074</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="Ellipse 24"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="542925" y="6267450"/>
+          <a:ext cx="2725874" cy="904875"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>20775</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="Ellipse 25"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4762500" y="4076700"/>
+          <a:ext cx="1440000" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>695324</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>41324</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>22275</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="Ellipse 26"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6115049" y="6686550"/>
+          <a:ext cx="108000" cy="108000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>184199</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>3225</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="Ellipse 27"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3209924" y="6667500"/>
+          <a:ext cx="108000" cy="108000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>689310</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>175460</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>104803</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>167466</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="Ellipse 28"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22947731" y="275723"/>
+          <a:ext cx="180000" cy="180000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>56175</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>46650</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="Ellipse 49"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2247900" y="1304925"/>
+          <a:ext cx="180000" cy="180000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>46650</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>56175</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="51" name="Ellipse 50"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2238375" y="3981450"/>
+          <a:ext cx="180000" cy="180000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>427650</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>46650</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="52" name="Ellipse 51"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2619375" y="6638925"/>
+          <a:ext cx="180000" cy="180000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>189525</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>56175</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="55" name="Ellipse 54"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5429250" y="1314450"/>
+          <a:ext cx="180000" cy="180000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>503850</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>56175</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="57" name="Ellipse 56"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5741194" y="6460331"/>
+          <a:ext cx="180000" cy="180000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>135074</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="58" name="Ellipse 57"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="540544" y="6079331"/>
+          <a:ext cx="2725874" cy="904875"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>20775</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="59" name="Ellipse 58"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4760119" y="6555581"/>
+          <a:ext cx="1440000" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>695324</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>41324</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>22275</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="60" name="Ellipse 59"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6112668" y="6498431"/>
+          <a:ext cx="108000" cy="108000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>184199</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>3225</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="61" name="Ellipse 60"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3207543" y="6479381"/>
+          <a:ext cx="108000" cy="108000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>427650</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>46650</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="62" name="Ellipse 61"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2616994" y="6450806"/>
+          <a:ext cx="180000" cy="180000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>503850</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>56175</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="63" name="Ellipse 62"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12743949" y="1294899"/>
+          <a:ext cx="180000" cy="177493"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>135074</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="64" name="Ellipse 63"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="544930" y="8538912"/>
+          <a:ext cx="2735901" cy="892342"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>36594</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>20775</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>87728</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="65" name="Ellipse 64"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11760367" y="1264818"/>
+          <a:ext cx="1445013" cy="239127"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>81213</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>17045</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>191719</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>122538</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="66" name="Ellipse 65"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12501312" y="1433262"/>
+          <a:ext cx="110506" cy="105493"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>201527</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>160922</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>309527</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>78422</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="67" name="Ellipse 66"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8799093" y="1765133"/>
+          <a:ext cx="108000" cy="105493"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>427650</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>46650</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="68" name="Ellipse 67"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2628900" y="8905374"/>
+          <a:ext cx="180000" cy="177493"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>503850</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>56175</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="69" name="Ellipse 68"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12743949" y="1294899"/>
+          <a:ext cx="180000" cy="177493"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>135074</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="70" name="Ellipse 69"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7525753" y="918912"/>
+          <a:ext cx="2735900" cy="892342"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>20775</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="71" name="Ellipse 70"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11760367" y="1390149"/>
+          <a:ext cx="1445013" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>695324</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>41324</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>22275</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="72" name="Ellipse 71"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13115423" y="1332999"/>
+          <a:ext cx="110506" cy="105493"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>184199</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>3225</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="73" name="Ellipse 72"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10202778" y="1313949"/>
+          <a:ext cx="108000" cy="105493"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>427650</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>46650</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="74" name="Ellipse 73"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9609722" y="1285374"/>
+          <a:ext cx="180000" cy="177493"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5744,6 +8367,169 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:M8"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="2" style="50" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="50" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="11.42578125" style="50"/>
+    <col min="7" max="7" width="13.85546875" style="50" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="11.42578125" style="50"/>
+    <col min="13" max="13" width="53.7109375" style="50" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="11.42578125" style="50"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:13">
+      <c r="B2" s="44" t="s">
+        <v>225</v>
+      </c>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="34" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13">
+      <c r="B3" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="51" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" s="51" t="s">
+        <v>117</v>
+      </c>
+      <c r="G3" s="51" t="s">
+        <v>230</v>
+      </c>
+      <c r="H3" s="52" t="s">
+        <v>140</v>
+      </c>
+      <c r="I3" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="53" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13">
+      <c r="B4" s="54" t="s">
+        <v>229</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>229</v>
+      </c>
+      <c r="D4" s="54" t="s">
+        <v>229</v>
+      </c>
+      <c r="E4" s="54" t="s">
+        <v>229</v>
+      </c>
+      <c r="F4" s="54" t="s">
+        <v>227</v>
+      </c>
+      <c r="G4" s="55" t="s">
+        <v>231</v>
+      </c>
+      <c r="H4" s="54" t="s">
+        <v>229</v>
+      </c>
+      <c r="I4" s="54" t="s">
+        <v>229</v>
+      </c>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="54"/>
+    </row>
+    <row r="5" spans="2:13">
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="54"/>
+    </row>
+    <row r="6" spans="2:13">
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="54"/>
+    </row>
+    <row r="7" spans="2:13">
+      <c r="B7" s="54"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="54"/>
+      <c r="M7" s="54"/>
+    </row>
+    <row r="8" spans="2:13">
+      <c r="B8" s="54"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="54"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7746,7 +10532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
@@ -7761,8 +10547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -7938,14 +10724,16 @@
       <c r="C14" s="37"/>
       <c r="D14" s="35"/>
     </row>
-    <row r="15" spans="1:11" ht="45">
+    <row r="15" spans="1:11" ht="75">
       <c r="A15" s="35" t="s">
         <v>228</v>
       </c>
       <c r="B15" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="C15" s="37"/>
+      <c r="C15" s="35" t="s">
+        <v>277</v>
+      </c>
       <c r="D15" s="35" t="s">
         <v>224</v>
       </c>
@@ -7964,7 +10752,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="60">
+    <row r="17" spans="1:5" ht="60">
       <c r="A17" s="37" t="s">
         <v>119</v>
       </c>
@@ -7978,7 +10766,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="75">
+    <row r="18" spans="1:5" ht="75">
       <c r="A18" s="37" t="s">
         <v>124</v>
       </c>
@@ -7992,7 +10780,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="45">
+    <row r="19" spans="1:5" ht="45">
       <c r="A19" s="37" t="s">
         <v>140</v>
       </c>
@@ -8006,7 +10794,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="18">
+    <row r="20" spans="1:5" ht="18">
       <c r="A20" s="72" t="s">
         <v>37</v>
       </c>
@@ -8018,7 +10806,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="48">
+    <row r="21" spans="1:5" ht="48">
       <c r="A21" s="37" t="s">
         <v>249</v>
       </c>
@@ -8030,7 +10818,7 @@
       </c>
       <c r="D21" s="35"/>
     </row>
-    <row r="22" spans="1:4" ht="30">
+    <row r="22" spans="1:5" ht="30">
       <c r="A22" s="35" t="s">
         <v>265</v>
       </c>
@@ -8042,7 +10830,7 @@
       </c>
       <c r="D22" s="35"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:5">
       <c r="A23" s="73" t="s">
         <v>148</v>
       </c>
@@ -8054,7 +10842,7 @@
       </c>
       <c r="D23" s="35"/>
     </row>
-    <row r="24" spans="1:4" ht="30">
+    <row r="24" spans="1:5" ht="30">
       <c r="A24" s="35" t="s">
         <v>71</v>
       </c>
@@ -8066,25 +10854,25 @@
       </c>
       <c r="D24" s="35"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:5">
       <c r="A25" s="37"/>
       <c r="B25" s="35"/>
       <c r="C25" s="35"/>
       <c r="D25" s="35"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5">
       <c r="A26" s="33"/>
       <c r="B26" s="33"/>
       <c r="C26" s="33"/>
       <c r="D26" s="33"/>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5">
       <c r="A27" s="33"/>
       <c r="B27" s="33"/>
       <c r="C27" s="33"/>
       <c r="D27" s="33"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:5">
       <c r="A28" s="57"/>
       <c r="B28" s="58" t="s">
         <v>165</v>
@@ -8096,7 +10884,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:5">
       <c r="A29" s="37"/>
       <c r="B29" s="35" t="s">
         <v>163</v>
@@ -8108,7 +10896,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="33">
+    <row r="30" spans="1:5" ht="33">
       <c r="A30" s="37"/>
       <c r="B30" s="35" t="s">
         <v>264</v>
@@ -8119,14 +10907,17 @@
       <c r="D30" s="35" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30" s="78" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="37"/>
       <c r="B31" s="37"/>
       <c r="C31" s="37"/>
       <c r="D31" s="37"/>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:5">
       <c r="A32" s="37"/>
       <c r="B32" s="37"/>
       <c r="C32" s="37"/>
@@ -8176,163 +10967,953 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:M8"/>
+  <dimension ref="B1:AD56"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2" style="50" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="50" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="11.42578125" style="50"/>
-    <col min="7" max="7" width="13.85546875" style="50" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="11.42578125" style="50"/>
-    <col min="13" max="13" width="53.7109375" style="50" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="11.42578125" style="50"/>
+    <col min="1" max="1" width="1.28515625" customWidth="1"/>
+    <col min="11" max="11" width="1.42578125" customWidth="1"/>
+    <col min="21" max="21" width="1.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13">
-      <c r="B2" s="44" t="s">
-        <v>225</v>
-      </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="47" t="s">
-        <v>226</v>
-      </c>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="34" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="3" spans="2:13">
-      <c r="B3" s="43" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" s="51" t="s">
+    <row r="1" spans="2:30" ht="8.25" customHeight="1"/>
+    <row r="2" spans="2:30">
+      <c r="B2" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="51" t="s">
+      <c r="C2" s="88" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="51" t="s">
+      <c r="D2" s="89" t="s">
         <v>115</v>
       </c>
-      <c r="F3" s="51" t="s">
-        <v>117</v>
-      </c>
-      <c r="G3" s="51" t="s">
-        <v>230</v>
-      </c>
-      <c r="H3" s="52" t="s">
+      <c r="E2" s="88" t="s">
         <v>140</v>
       </c>
-      <c r="I3" s="52" t="s">
+      <c r="F2" s="90" t="s">
         <v>114</v>
       </c>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="53" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13">
-      <c r="B4" s="54" t="s">
-        <v>229</v>
-      </c>
-      <c r="C4" s="54" t="s">
-        <v>229</v>
-      </c>
-      <c r="D4" s="54" t="s">
-        <v>229</v>
-      </c>
-      <c r="E4" s="54" t="s">
-        <v>229</v>
-      </c>
-      <c r="F4" s="54" t="s">
-        <v>227</v>
-      </c>
-      <c r="G4" s="55" t="s">
-        <v>231</v>
-      </c>
-      <c r="H4" s="54" t="s">
-        <v>229</v>
-      </c>
-      <c r="I4" s="54" t="s">
-        <v>229</v>
-      </c>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="54"/>
-      <c r="M4" s="54"/>
-    </row>
-    <row r="5" spans="2:13">
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="54"/>
-      <c r="K5" s="54"/>
-      <c r="L5" s="54"/>
-      <c r="M5" s="54"/>
-    </row>
-    <row r="6" spans="2:13">
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="54"/>
-      <c r="M6" s="54"/>
-    </row>
-    <row r="7" spans="2:13">
-      <c r="B7" s="54"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="54"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="54"/>
-      <c r="L7" s="54"/>
-      <c r="M7" s="54"/>
-    </row>
-    <row r="8" spans="2:13">
-      <c r="B8" s="54"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="54"/>
-      <c r="J8" s="54"/>
-      <c r="K8" s="54"/>
-      <c r="L8" s="54"/>
-      <c r="M8" s="54"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="80"/>
+      <c r="L2" s="98" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="100" t="s">
+        <v>46</v>
+      </c>
+      <c r="N2" s="89" t="s">
+        <v>115</v>
+      </c>
+      <c r="O2" s="88" t="s">
+        <v>140</v>
+      </c>
+      <c r="P2" s="90" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q2" s="79"/>
+      <c r="R2" s="79"/>
+      <c r="S2" s="79"/>
+      <c r="T2" s="80"/>
+      <c r="V2" s="96" t="s">
+        <v>45</v>
+      </c>
+      <c r="W2" s="88" t="s">
+        <v>46</v>
+      </c>
+      <c r="X2" s="89" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y2" s="88" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z2" s="90" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA2" s="79"/>
+      <c r="AB2" s="79"/>
+      <c r="AC2" s="79"/>
+      <c r="AD2" s="80"/>
+    </row>
+    <row r="3" spans="2:30">
+      <c r="B3" s="91">
+        <v>0</v>
+      </c>
+      <c r="C3" s="92">
+        <v>90</v>
+      </c>
+      <c r="D3" s="92">
+        <v>0</v>
+      </c>
+      <c r="E3" s="92">
+        <v>0</v>
+      </c>
+      <c r="F3" s="93">
+        <v>0</v>
+      </c>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="82"/>
+      <c r="L3" s="99">
+        <v>0.5</v>
+      </c>
+      <c r="M3" s="101">
+        <v>85</v>
+      </c>
+      <c r="N3" s="92">
+        <v>0</v>
+      </c>
+      <c r="O3" s="92">
+        <v>0</v>
+      </c>
+      <c r="P3" s="93">
+        <v>270</v>
+      </c>
+      <c r="Q3" s="81"/>
+      <c r="R3" s="81"/>
+      <c r="S3" s="81"/>
+      <c r="T3" s="82"/>
+      <c r="V3" s="97">
+        <v>0.5</v>
+      </c>
+      <c r="W3" s="92">
+        <v>90</v>
+      </c>
+      <c r="X3" s="92">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="92">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="93">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="81"/>
+      <c r="AB3" s="81"/>
+      <c r="AC3" s="81"/>
+      <c r="AD3" s="82"/>
+    </row>
+    <row r="4" spans="2:30">
+      <c r="B4" s="83"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="82"/>
+      <c r="L4" s="83"/>
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="81"/>
+      <c r="S4" s="81"/>
+      <c r="T4" s="82"/>
+      <c r="V4" s="83"/>
+      <c r="W4" s="81"/>
+      <c r="X4" s="81"/>
+      <c r="Y4" s="81"/>
+      <c r="Z4" s="81"/>
+      <c r="AA4" s="81"/>
+      <c r="AB4" s="81"/>
+      <c r="AC4" s="81"/>
+      <c r="AD4" s="82"/>
+    </row>
+    <row r="5" spans="2:30">
+      <c r="B5" s="83"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="82"/>
+      <c r="L5" s="83"/>
+      <c r="M5" s="81"/>
+      <c r="N5" s="81"/>
+      <c r="O5" s="81"/>
+      <c r="P5" s="81"/>
+      <c r="Q5" s="81"/>
+      <c r="R5" s="81"/>
+      <c r="S5" s="81"/>
+      <c r="T5" s="82"/>
+      <c r="V5" s="83"/>
+      <c r="W5" s="81"/>
+      <c r="X5" s="81"/>
+      <c r="Y5" s="81"/>
+      <c r="Z5" s="81"/>
+      <c r="AA5" s="81"/>
+      <c r="AB5" s="81"/>
+      <c r="AC5" s="81"/>
+      <c r="AD5" s="82"/>
+    </row>
+    <row r="6" spans="2:30">
+      <c r="B6" s="83"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="81"/>
+      <c r="F6" s="81"/>
+      <c r="G6" s="81"/>
+      <c r="H6" s="81"/>
+      <c r="I6" s="81"/>
+      <c r="J6" s="82"/>
+      <c r="L6" s="83"/>
+      <c r="M6" s="81"/>
+      <c r="N6" s="81"/>
+      <c r="O6" s="81"/>
+      <c r="P6" s="81"/>
+      <c r="Q6" s="81"/>
+      <c r="R6" s="81"/>
+      <c r="S6" s="81"/>
+      <c r="T6" s="82"/>
+      <c r="V6" s="83"/>
+      <c r="W6" s="81"/>
+      <c r="X6" s="81"/>
+      <c r="Y6" s="81"/>
+      <c r="Z6" s="81"/>
+      <c r="AA6" s="81"/>
+      <c r="AB6" s="81"/>
+      <c r="AC6" s="81"/>
+      <c r="AD6" s="82"/>
+    </row>
+    <row r="7" spans="2:30">
+      <c r="B7" s="83"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="81"/>
+      <c r="H7" s="81"/>
+      <c r="I7" s="81"/>
+      <c r="J7" s="82"/>
+      <c r="L7" s="83"/>
+      <c r="M7" s="81"/>
+      <c r="N7" s="81"/>
+      <c r="O7" s="81"/>
+      <c r="P7" s="81"/>
+      <c r="Q7" s="81"/>
+      <c r="R7" s="81"/>
+      <c r="S7" s="81"/>
+      <c r="T7" s="82"/>
+      <c r="V7" s="83"/>
+      <c r="W7" s="81"/>
+      <c r="X7" s="81"/>
+      <c r="Y7" s="81"/>
+      <c r="Z7" s="81"/>
+      <c r="AA7" s="81"/>
+      <c r="AB7" s="81"/>
+      <c r="AC7" s="81"/>
+      <c r="AD7" s="82"/>
+    </row>
+    <row r="8" spans="2:30">
+      <c r="B8" s="83"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="81"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="82"/>
+      <c r="L8" s="83"/>
+      <c r="M8" s="81"/>
+      <c r="N8" s="81"/>
+      <c r="O8" s="81"/>
+      <c r="P8" s="81" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q8" s="81"/>
+      <c r="R8" s="81"/>
+      <c r="S8" s="81"/>
+      <c r="T8" s="82"/>
+      <c r="V8" s="83"/>
+      <c r="W8" s="81"/>
+      <c r="X8" s="81"/>
+      <c r="Y8" s="81"/>
+      <c r="Z8" s="81"/>
+      <c r="AA8" s="81"/>
+      <c r="AB8" s="81"/>
+      <c r="AC8" s="81"/>
+      <c r="AD8" s="82"/>
+    </row>
+    <row r="9" spans="2:30">
+      <c r="B9" s="83"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="81"/>
+      <c r="F9" s="81"/>
+      <c r="G9" s="81"/>
+      <c r="H9" s="81"/>
+      <c r="I9" s="81"/>
+      <c r="J9" s="82"/>
+      <c r="L9" s="83"/>
+      <c r="M9" s="81"/>
+      <c r="N9" s="81"/>
+      <c r="O9" s="81"/>
+      <c r="P9" s="81"/>
+      <c r="Q9" s="81"/>
+      <c r="R9" s="81"/>
+      <c r="S9" s="81"/>
+      <c r="T9" s="82"/>
+      <c r="V9" s="83"/>
+      <c r="W9" s="81"/>
+      <c r="X9" s="81"/>
+      <c r="Y9" s="81"/>
+      <c r="Z9" s="81"/>
+      <c r="AA9" s="81"/>
+      <c r="AB9" s="81"/>
+      <c r="AC9" s="81"/>
+      <c r="AD9" s="82"/>
+    </row>
+    <row r="10" spans="2:30">
+      <c r="B10" s="83"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="81"/>
+      <c r="H10" s="81"/>
+      <c r="I10" s="81"/>
+      <c r="J10" s="82"/>
+      <c r="L10" s="83"/>
+      <c r="M10" s="81"/>
+      <c r="N10" s="81"/>
+      <c r="O10" s="81"/>
+      <c r="P10" s="81"/>
+      <c r="Q10" s="81"/>
+      <c r="R10" s="81"/>
+      <c r="S10" s="81"/>
+      <c r="T10" s="82"/>
+      <c r="V10" s="83"/>
+      <c r="W10" s="81"/>
+      <c r="X10" s="81"/>
+      <c r="Y10" s="81"/>
+      <c r="Z10" s="81"/>
+      <c r="AA10" s="81"/>
+      <c r="AB10" s="81"/>
+      <c r="AC10" s="81"/>
+      <c r="AD10" s="82"/>
+    </row>
+    <row r="11" spans="2:30">
+      <c r="B11" s="83"/>
+      <c r="C11" s="81"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="81"/>
+      <c r="I11" s="81"/>
+      <c r="J11" s="82"/>
+      <c r="L11" s="83"/>
+      <c r="M11" s="81"/>
+      <c r="N11" s="81"/>
+      <c r="O11" s="81"/>
+      <c r="P11" s="81"/>
+      <c r="Q11" s="81"/>
+      <c r="R11" s="81"/>
+      <c r="S11" s="81"/>
+      <c r="T11" s="82"/>
+      <c r="V11" s="83"/>
+      <c r="W11" s="81"/>
+      <c r="X11" s="81"/>
+      <c r="Y11" s="81"/>
+      <c r="Z11" s="81"/>
+      <c r="AA11" s="81"/>
+      <c r="AB11" s="81"/>
+      <c r="AC11" s="81"/>
+      <c r="AD11" s="82"/>
+    </row>
+    <row r="12" spans="2:30">
+      <c r="B12" s="83"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="81"/>
+      <c r="F12" s="81"/>
+      <c r="G12" s="81"/>
+      <c r="H12" s="81"/>
+      <c r="I12" s="81"/>
+      <c r="J12" s="82"/>
+      <c r="L12" s="83"/>
+      <c r="M12" s="81"/>
+      <c r="N12" s="81"/>
+      <c r="O12" s="81"/>
+      <c r="P12" s="81"/>
+      <c r="Q12" s="81"/>
+      <c r="R12" s="81"/>
+      <c r="S12" s="81"/>
+      <c r="T12" s="82"/>
+      <c r="V12" s="83"/>
+      <c r="W12" s="81"/>
+      <c r="X12" s="81"/>
+      <c r="Y12" s="81"/>
+      <c r="Z12" s="81"/>
+      <c r="AA12" s="81"/>
+      <c r="AB12" s="81"/>
+      <c r="AC12" s="81"/>
+      <c r="AD12" s="82"/>
+    </row>
+    <row r="13" spans="2:30">
+      <c r="B13" s="83"/>
+      <c r="C13" s="81"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="81"/>
+      <c r="F13" s="81"/>
+      <c r="G13" s="81"/>
+      <c r="H13" s="81"/>
+      <c r="I13" s="81"/>
+      <c r="J13" s="82"/>
+      <c r="L13" s="83"/>
+      <c r="M13" s="81"/>
+      <c r="N13" s="81"/>
+      <c r="O13" s="81"/>
+      <c r="P13" s="81"/>
+      <c r="Q13" s="81"/>
+      <c r="R13" s="81"/>
+      <c r="S13" s="81"/>
+      <c r="T13" s="82"/>
+      <c r="V13" s="83"/>
+      <c r="W13" s="81"/>
+      <c r="X13" s="81"/>
+      <c r="Y13" s="81"/>
+      <c r="Z13" s="81"/>
+      <c r="AA13" s="81"/>
+      <c r="AB13" s="81"/>
+      <c r="AC13" s="81"/>
+      <c r="AD13" s="82"/>
+    </row>
+    <row r="14" spans="2:30">
+      <c r="B14" s="84"/>
+      <c r="C14" s="85"/>
+      <c r="D14" s="85"/>
+      <c r="E14" s="85"/>
+      <c r="F14" s="85"/>
+      <c r="G14" s="85"/>
+      <c r="H14" s="85"/>
+      <c r="I14" s="85"/>
+      <c r="J14" s="86"/>
+      <c r="L14" s="84"/>
+      <c r="M14" s="85"/>
+      <c r="N14" s="85"/>
+      <c r="O14" s="85"/>
+      <c r="P14" s="85"/>
+      <c r="Q14" s="85"/>
+      <c r="R14" s="85"/>
+      <c r="S14" s="85"/>
+      <c r="T14" s="86"/>
+      <c r="V14" s="84"/>
+      <c r="W14" s="85"/>
+      <c r="X14" s="85"/>
+      <c r="Y14" s="85"/>
+      <c r="Z14" s="85"/>
+      <c r="AA14" s="85"/>
+      <c r="AB14" s="85"/>
+      <c r="AC14" s="85"/>
+      <c r="AD14" s="86"/>
+    </row>
+    <row r="15" spans="2:30" ht="7.5" customHeight="1"/>
+    <row r="16" spans="2:30">
+      <c r="B16" s="87" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="88" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="89" t="s">
+        <v>115</v>
+      </c>
+      <c r="E16" s="88" t="s">
+        <v>140</v>
+      </c>
+      <c r="F16" s="94" t="s">
+        <v>114</v>
+      </c>
+      <c r="G16" s="79"/>
+      <c r="H16" s="79"/>
+      <c r="I16" s="79"/>
+      <c r="J16" s="80"/>
+    </row>
+    <row r="17" spans="2:10">
+      <c r="B17" s="91">
+        <v>0</v>
+      </c>
+      <c r="C17" s="92">
+        <v>90</v>
+      </c>
+      <c r="D17" s="92">
+        <v>0</v>
+      </c>
+      <c r="E17" s="92">
+        <v>0</v>
+      </c>
+      <c r="F17" s="95">
+        <v>90</v>
+      </c>
+      <c r="G17" s="81"/>
+      <c r="H17" s="81"/>
+      <c r="I17" s="81"/>
+      <c r="J17" s="82"/>
+    </row>
+    <row r="18" spans="2:10">
+      <c r="B18" s="83"/>
+      <c r="C18" s="81"/>
+      <c r="D18" s="81"/>
+      <c r="E18" s="81"/>
+      <c r="F18" s="81"/>
+      <c r="G18" s="81"/>
+      <c r="H18" s="81"/>
+      <c r="I18" s="81"/>
+      <c r="J18" s="82"/>
+    </row>
+    <row r="19" spans="2:10">
+      <c r="B19" s="83"/>
+      <c r="C19" s="81"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="81"/>
+      <c r="F19" s="81"/>
+      <c r="G19" s="81"/>
+      <c r="H19" s="81"/>
+      <c r="I19" s="81"/>
+      <c r="J19" s="82"/>
+    </row>
+    <row r="20" spans="2:10">
+      <c r="B20" s="83"/>
+      <c r="C20" s="81"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="81"/>
+      <c r="F20" s="81"/>
+      <c r="G20" s="81"/>
+      <c r="H20" s="81"/>
+      <c r="I20" s="81"/>
+      <c r="J20" s="82"/>
+    </row>
+    <row r="21" spans="2:10">
+      <c r="B21" s="83"/>
+      <c r="C21" s="81"/>
+      <c r="D21" s="81"/>
+      <c r="E21" s="81"/>
+      <c r="F21" s="81"/>
+      <c r="G21" s="81"/>
+      <c r="H21" s="81"/>
+      <c r="I21" s="81"/>
+      <c r="J21" s="82"/>
+    </row>
+    <row r="22" spans="2:10">
+      <c r="B22" s="83"/>
+      <c r="C22" s="81"/>
+      <c r="D22" s="81"/>
+      <c r="E22" s="81"/>
+      <c r="F22" s="81"/>
+      <c r="G22" s="81"/>
+      <c r="H22" s="81"/>
+      <c r="I22" s="81"/>
+      <c r="J22" s="82"/>
+    </row>
+    <row r="23" spans="2:10">
+      <c r="B23" s="83"/>
+      <c r="C23" s="81"/>
+      <c r="D23" s="81"/>
+      <c r="E23" s="81"/>
+      <c r="F23" s="81"/>
+      <c r="G23" s="81"/>
+      <c r="H23" s="81"/>
+      <c r="I23" s="81"/>
+      <c r="J23" s="82"/>
+    </row>
+    <row r="24" spans="2:10">
+      <c r="B24" s="83"/>
+      <c r="C24" s="81"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="81"/>
+      <c r="G24" s="81"/>
+      <c r="H24" s="81"/>
+      <c r="I24" s="81"/>
+      <c r="J24" s="82"/>
+    </row>
+    <row r="25" spans="2:10">
+      <c r="B25" s="83"/>
+      <c r="C25" s="81"/>
+      <c r="D25" s="81"/>
+      <c r="E25" s="81"/>
+      <c r="F25" s="81"/>
+      <c r="G25" s="81"/>
+      <c r="H25" s="81"/>
+      <c r="I25" s="81"/>
+      <c r="J25" s="82"/>
+    </row>
+    <row r="26" spans="2:10">
+      <c r="B26" s="83"/>
+      <c r="C26" s="81"/>
+      <c r="D26" s="81"/>
+      <c r="E26" s="81"/>
+      <c r="F26" s="81"/>
+      <c r="G26" s="81"/>
+      <c r="H26" s="81"/>
+      <c r="I26" s="81"/>
+      <c r="J26" s="82"/>
+    </row>
+    <row r="27" spans="2:10">
+      <c r="B27" s="83"/>
+      <c r="C27" s="81"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="81"/>
+      <c r="F27" s="81"/>
+      <c r="G27" s="81"/>
+      <c r="H27" s="81"/>
+      <c r="I27" s="81"/>
+      <c r="J27" s="82"/>
+    </row>
+    <row r="28" spans="2:10">
+      <c r="B28" s="84"/>
+      <c r="C28" s="85"/>
+      <c r="D28" s="85"/>
+      <c r="E28" s="85"/>
+      <c r="F28" s="85"/>
+      <c r="G28" s="85"/>
+      <c r="H28" s="85"/>
+      <c r="I28" s="85"/>
+      <c r="J28" s="86"/>
+    </row>
+    <row r="29" spans="2:10" ht="7.5" customHeight="1"/>
+    <row r="30" spans="2:10">
+      <c r="B30" s="96" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="88" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="89" t="s">
+        <v>115</v>
+      </c>
+      <c r="E30" s="88" t="s">
+        <v>140</v>
+      </c>
+      <c r="F30" s="90" t="s">
+        <v>114</v>
+      </c>
+      <c r="G30" s="79"/>
+      <c r="H30" s="79"/>
+      <c r="I30" s="79"/>
+      <c r="J30" s="80"/>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="B31" s="97">
+        <v>0.5</v>
+      </c>
+      <c r="C31" s="92">
+        <v>90</v>
+      </c>
+      <c r="D31" s="92">
+        <v>0</v>
+      </c>
+      <c r="E31" s="92">
+        <v>0</v>
+      </c>
+      <c r="F31" s="93">
+        <v>0</v>
+      </c>
+      <c r="G31" s="81"/>
+      <c r="H31" s="81"/>
+      <c r="I31" s="81"/>
+      <c r="J31" s="82"/>
+    </row>
+    <row r="32" spans="2:10">
+      <c r="B32" s="83"/>
+      <c r="C32" s="81"/>
+      <c r="D32" s="81"/>
+      <c r="E32" s="81"/>
+      <c r="F32" s="81"/>
+      <c r="G32" s="81"/>
+      <c r="H32" s="81"/>
+      <c r="I32" s="81"/>
+      <c r="J32" s="82"/>
+    </row>
+    <row r="33" spans="2:10">
+      <c r="B33" s="83"/>
+      <c r="C33" s="81"/>
+      <c r="D33" s="81"/>
+      <c r="E33" s="81"/>
+      <c r="F33" s="81"/>
+      <c r="G33" s="81"/>
+      <c r="H33" s="81"/>
+      <c r="I33" s="81"/>
+      <c r="J33" s="82"/>
+    </row>
+    <row r="34" spans="2:10">
+      <c r="B34" s="83"/>
+      <c r="C34" s="81"/>
+      <c r="D34" s="81"/>
+      <c r="E34" s="81"/>
+      <c r="F34" s="81"/>
+      <c r="G34" s="81"/>
+      <c r="H34" s="81"/>
+      <c r="I34" s="81"/>
+      <c r="J34" s="82"/>
+    </row>
+    <row r="35" spans="2:10">
+      <c r="B35" s="83"/>
+      <c r="C35" s="81"/>
+      <c r="D35" s="81"/>
+      <c r="E35" s="81"/>
+      <c r="F35" s="81"/>
+      <c r="G35" s="81"/>
+      <c r="H35" s="81"/>
+      <c r="I35" s="81"/>
+      <c r="J35" s="82"/>
+    </row>
+    <row r="36" spans="2:10">
+      <c r="B36" s="83"/>
+      <c r="C36" s="81"/>
+      <c r="D36" s="81"/>
+      <c r="E36" s="81"/>
+      <c r="F36" s="81"/>
+      <c r="G36" s="81"/>
+      <c r="H36" s="81"/>
+      <c r="I36" s="81"/>
+      <c r="J36" s="82"/>
+    </row>
+    <row r="37" spans="2:10">
+      <c r="B37" s="83"/>
+      <c r="C37" s="81"/>
+      <c r="D37" s="81"/>
+      <c r="E37" s="81"/>
+      <c r="F37" s="81"/>
+      <c r="G37" s="81"/>
+      <c r="H37" s="81"/>
+      <c r="I37" s="81"/>
+      <c r="J37" s="82"/>
+    </row>
+    <row r="38" spans="2:10">
+      <c r="B38" s="83"/>
+      <c r="C38" s="81"/>
+      <c r="D38" s="81"/>
+      <c r="E38" s="81"/>
+      <c r="F38" s="81"/>
+      <c r="G38" s="81"/>
+      <c r="H38" s="81"/>
+      <c r="I38" s="81"/>
+      <c r="J38" s="82"/>
+    </row>
+    <row r="39" spans="2:10">
+      <c r="B39" s="83"/>
+      <c r="C39" s="81"/>
+      <c r="D39" s="81"/>
+      <c r="E39" s="81"/>
+      <c r="F39" s="81"/>
+      <c r="G39" s="81"/>
+      <c r="H39" s="81"/>
+      <c r="I39" s="81"/>
+      <c r="J39" s="82"/>
+    </row>
+    <row r="40" spans="2:10">
+      <c r="B40" s="83"/>
+      <c r="C40" s="81"/>
+      <c r="D40" s="81"/>
+      <c r="E40" s="81"/>
+      <c r="F40" s="81"/>
+      <c r="G40" s="81"/>
+      <c r="H40" s="81"/>
+      <c r="I40" s="81"/>
+      <c r="J40" s="82"/>
+    </row>
+    <row r="41" spans="2:10">
+      <c r="B41" s="83"/>
+      <c r="C41" s="81"/>
+      <c r="D41" s="81"/>
+      <c r="E41" s="81"/>
+      <c r="F41" s="81"/>
+      <c r="G41" s="81"/>
+      <c r="H41" s="81"/>
+      <c r="I41" s="81"/>
+      <c r="J41" s="82"/>
+    </row>
+    <row r="42" spans="2:10">
+      <c r="B42" s="84"/>
+      <c r="C42" s="85"/>
+      <c r="D42" s="85"/>
+      <c r="E42" s="85"/>
+      <c r="F42" s="85"/>
+      <c r="G42" s="85"/>
+      <c r="H42" s="85"/>
+      <c r="I42" s="85"/>
+      <c r="J42" s="86"/>
+    </row>
+    <row r="43" spans="2:10" ht="6.75" customHeight="1"/>
+    <row r="44" spans="2:10">
+      <c r="B44" s="96" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" s="88" t="s">
+        <v>46</v>
+      </c>
+      <c r="D44" s="89" t="s">
+        <v>115</v>
+      </c>
+      <c r="E44" s="88" t="s">
+        <v>140</v>
+      </c>
+      <c r="F44" s="90" t="s">
+        <v>114</v>
+      </c>
+      <c r="G44" s="79"/>
+      <c r="H44" s="79"/>
+      <c r="I44" s="79"/>
+      <c r="J44" s="80"/>
+    </row>
+    <row r="45" spans="2:10">
+      <c r="B45" s="97">
+        <v>0.5</v>
+      </c>
+      <c r="C45" s="92">
+        <v>90</v>
+      </c>
+      <c r="D45" s="92">
+        <v>0</v>
+      </c>
+      <c r="E45" s="92">
+        <v>0</v>
+      </c>
+      <c r="F45" s="93">
+        <v>0</v>
+      </c>
+      <c r="G45" s="81"/>
+      <c r="H45" s="81"/>
+      <c r="I45" s="81"/>
+      <c r="J45" s="82"/>
+    </row>
+    <row r="46" spans="2:10">
+      <c r="B46" s="83"/>
+      <c r="C46" s="81"/>
+      <c r="D46" s="81"/>
+      <c r="E46" s="81"/>
+      <c r="F46" s="81"/>
+      <c r="G46" s="81"/>
+      <c r="H46" s="81"/>
+      <c r="I46" s="81"/>
+      <c r="J46" s="82"/>
+    </row>
+    <row r="47" spans="2:10">
+      <c r="B47" s="83"/>
+      <c r="C47" s="81"/>
+      <c r="D47" s="81"/>
+      <c r="E47" s="81"/>
+      <c r="F47" s="81"/>
+      <c r="G47" s="81"/>
+      <c r="H47" s="81"/>
+      <c r="I47" s="81"/>
+      <c r="J47" s="82"/>
+    </row>
+    <row r="48" spans="2:10">
+      <c r="B48" s="83"/>
+      <c r="C48" s="81"/>
+      <c r="D48" s="81"/>
+      <c r="E48" s="81"/>
+      <c r="F48" s="81"/>
+      <c r="G48" s="81"/>
+      <c r="H48" s="81"/>
+      <c r="I48" s="81"/>
+      <c r="J48" s="82"/>
+    </row>
+    <row r="49" spans="2:10">
+      <c r="B49" s="83"/>
+      <c r="C49" s="81"/>
+      <c r="D49" s="81"/>
+      <c r="E49" s="81"/>
+      <c r="F49" s="81"/>
+      <c r="G49" s="81"/>
+      <c r="H49" s="81"/>
+      <c r="I49" s="81"/>
+      <c r="J49" s="82"/>
+    </row>
+    <row r="50" spans="2:10">
+      <c r="B50" s="83"/>
+      <c r="C50" s="81"/>
+      <c r="D50" s="81"/>
+      <c r="E50" s="81"/>
+      <c r="F50" s="81"/>
+      <c r="G50" s="81"/>
+      <c r="H50" s="81"/>
+      <c r="I50" s="81"/>
+      <c r="J50" s="82"/>
+    </row>
+    <row r="51" spans="2:10">
+      <c r="B51" s="83"/>
+      <c r="C51" s="81"/>
+      <c r="D51" s="81"/>
+      <c r="E51" s="81"/>
+      <c r="F51" s="81"/>
+      <c r="G51" s="81"/>
+      <c r="H51" s="81"/>
+      <c r="I51" s="81"/>
+      <c r="J51" s="82"/>
+    </row>
+    <row r="52" spans="2:10">
+      <c r="B52" s="83"/>
+      <c r="C52" s="81"/>
+      <c r="D52" s="81"/>
+      <c r="E52" s="81"/>
+      <c r="F52" s="81"/>
+      <c r="G52" s="81"/>
+      <c r="H52" s="81"/>
+      <c r="I52" s="81"/>
+      <c r="J52" s="82"/>
+    </row>
+    <row r="53" spans="2:10">
+      <c r="B53" s="83"/>
+      <c r="C53" s="81"/>
+      <c r="D53" s="81"/>
+      <c r="E53" s="81"/>
+      <c r="F53" s="81"/>
+      <c r="G53" s="81"/>
+      <c r="H53" s="81"/>
+      <c r="I53" s="81"/>
+      <c r="J53" s="82"/>
+    </row>
+    <row r="54" spans="2:10">
+      <c r="B54" s="83"/>
+      <c r="C54" s="81"/>
+      <c r="D54" s="81"/>
+      <c r="E54" s="81"/>
+      <c r="F54" s="81"/>
+      <c r="G54" s="81"/>
+      <c r="H54" s="81"/>
+      <c r="I54" s="81"/>
+      <c r="J54" s="82"/>
+    </row>
+    <row r="55" spans="2:10">
+      <c r="B55" s="83"/>
+      <c r="C55" s="81"/>
+      <c r="D55" s="81"/>
+      <c r="E55" s="81"/>
+      <c r="F55" s="81"/>
+      <c r="G55" s="81"/>
+      <c r="H55" s="81"/>
+      <c r="I55" s="81"/>
+      <c r="J55" s="82"/>
+    </row>
+    <row r="56" spans="2:10">
+      <c r="B56" s="84"/>
+      <c r="C56" s="85"/>
+      <c r="D56" s="85"/>
+      <c r="E56" s="85"/>
+      <c r="F56" s="85"/>
+      <c r="G56" s="85"/>
+      <c r="H56" s="85"/>
+      <c r="I56" s="85"/>
+      <c r="J56" s="86"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="M3" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>